<commit_message>
- Requirement added - TCS-Inloggningsfucktion updated
</commit_message>
<xml_diff>
--- a/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
+++ b/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studies\Testautomation_CI_CD\InlämningsUppgift_TA\Del_1-Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9774C622-CF77-4457-9CE4-1A6DF12B55F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C119EC5A-77D1-4C95-998D-A94F6349072E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
+    <workbookView xWindow="1185" yWindow="3495" windowWidth="21600" windowHeight="11235" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Test case ID </t>
   </si>
@@ -60,16 +60,33 @@
   </si>
   <si>
     <t>Test specification- inloggningsfunktion</t>
+  </si>
+  <si>
+    <t>Del 2 – Inloggningsfunktion</t>
+  </si>
+  <si>
+    <t>Req link</t>
+  </si>
+  <si>
+    <t>Req Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,16 +109,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -434,26 +454,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BBF6A0-D8E2-406A-AD12-25A43EEED0E6}">
-  <dimension ref="B2:L4"/>
+  <dimension ref="B2:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:L2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -461,34 +482,49 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="E2:M2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{0D70471D-5F48-46BB-A16F-FCF8C9ECB572}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test specs inloggningsfunktion updated
</commit_message>
<xml_diff>
--- a/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
+++ b/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studies\Testautomation_CI_CD\InlämningsUppgift_TA\Del_1-Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C65CE8F-704C-490A-BF30-2C9BFF3BB112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0425573-DDA0-402A-A496-035841F7192C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25485" yWindow="2040" windowWidth="21600" windowHeight="11235" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Test case ID </t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Req Link</t>
+  </si>
+  <si>
+    <t>Test Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version </t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>IDE</t>
   </si>
 </sst>
 </file>
@@ -115,10 +127,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -454,37 +466,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BBF6A0-D8E2-406A-AD12-25A43EEED0E6}">
-  <dimension ref="B2:M5"/>
+  <dimension ref="B2:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -501,26 +522,38 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:M2"/>
+    <mergeCell ref="E2:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{0D70471D-5F48-46BB-A16F-FCF8C9ECB572}"/>

</xml_diff>

<commit_message>
Test specification inloggningsfunktion updated
</commit_message>
<xml_diff>
--- a/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
+++ b/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studies\Testautomation_CI_CD\InlämningsUppgift_TA\Del_1-Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0425573-DDA0-402A-A496-035841F7192C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E184918-8B12-4AD7-BCD5-7EDF25989081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25485" yWindow="2040" windowWidth="21600" windowHeight="11235" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
   <si>
     <t xml:space="preserve">Test case ID </t>
   </si>
@@ -71,23 +71,320 @@
     <t>Req Link</t>
   </si>
   <si>
-    <t>Test Environment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version </t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>IDE</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fixture som ansvarar för setup och teardown av WebDriver.
+ Detta gör testerna oberoende av varandra, vilket är viktigt i CI-miljöer.
+   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python 3.13.7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Environment </t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python version </t>
+  </si>
+  <si>
+    <t>PyCharm 2025.2.5
+Community Edition</t>
+  </si>
+  <si>
+    <t>Microsoft Windows
+ [Version 10.0.26200.7462]</t>
+  </si>
+  <si>
+    <t>Test framwork-1</t>
+  </si>
+  <si>
+    <t>Pytest
+[pytest-9.0]</t>
+  </si>
+  <si>
+    <t>Test framwork-2</t>
+  </si>
+  <si>
+    <t>Selenium 
+[4.39.0]</t>
+  </si>
+  <si>
+    <t>Version control system</t>
+  </si>
+  <si>
+    <t>Code Hosting Platform</t>
+  </si>
+  <si>
+    <t>git 
+[version 2.47.1.windows.1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitHub
+</t>
+  </si>
+  <si>
+    <t>CI/CD</t>
+  </si>
+  <si>
+    <t>GitHub Actions</t>
+  </si>
+  <si>
+    <t>En Chrome-webbläsare startas i headless-läge
+Webbläsaren öppnar den angivna URL:en
+Testerna körs med en fungerande WebDriver
+Webbläsaren stängs korrekt efter varje test
+Inga webbläsarprocesser lämnas kvar (viktigt i CI)</t>
+  </si>
+  <si>
+    <t>Koden uppfyller
+de förväntade resultaten</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>def login(driver, username, password):</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hjälpfunktion för inloggning.
+ Minskar kodduplicering och gör testerna mer lättlästa.
+   </t>
+  </si>
+  <si>
+    <t>Def driver():</t>
+  </si>
+  <si>
+    <t>Fält fylls i korrekt
+Inloggningsknappen klickas
+Inloggningsprocessen initieras
+Förväntade resultat uppnås om sidan och element finns</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>def test_successful_login_username1(driver):</t>
+  </si>
+  <si>
+    <t>Användare lyckats att logga
+ in med giltiga uppgifter. 
+(username: standard_user,
+password: secret_sauce)</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>def test_successful_login_username2(driver):</t>
+  </si>
+  <si>
+    <t>Användare lyckats att logga
+ in med giltiga uppgifter. 
+(username: problem_user,
+password: secret_sauce)</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>def test_successful_login_username3(driver):</t>
+  </si>
+  <si>
+    <t>Användare lyckats att logga
+ in med giltiga uppgifter. 
+(username: performance_glitch_user,
+password: secret_sauce)</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>def test_successful_login_username4(driver):</t>
+  </si>
+  <si>
+    <t>Användare lyckats att logga
+ in med giltiga uppgifter. 
+(username: error_user,
+password: secret_sauce)</t>
+  </si>
+  <si>
+    <t>Verifierar att användaren kan logga in med giltiga uppgifter.
+Detta är ett kritiskt användarflöde och lämpar sig väl för Selenium-testning.</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>def test_successful_login_username5(driver):</t>
+  </si>
+  <si>
+    <t>Användare lyckats att logga
+ in med giltiga uppgifter. 
+(username: visual_user,
+password: secret_sauce)</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>def test_wrong_password_username1(driver):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Säkerställer att systemet blockerar inloggning vid fel lösenord
+och ger användaren korrekt feedback.
+ </t>
+  </si>
+  <si>
+    <t>Användare lyckats inte att logga
+ in med fel lösenord. 
+(username: standard_user,
+password: wrong_password)</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>def test_wrong_password_username2(driver):</t>
+  </si>
+  <si>
+    <t>Säkerställer att systemet blockerar inloggning vid fel lösenord
+och ger användaren korrekt feedback.</t>
+  </si>
+  <si>
+    <t>Användare lyckats inte att logga
+ in med fel lösenord. 
+(username: problem_user,
+password: wrong_password)</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>def test_wrong_password_username3(driver):</t>
+  </si>
+  <si>
+    <t>Användare lyckats inte att logga
+ in med fel lösenord. 
+(username:  performance_glitch_user,
+password: wrong_password)</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>def test_wrong_password_username4(driver):</t>
+  </si>
+  <si>
+    <t>Användare lyckats inte att logga
+ in med fel lösenord. 
+(username:  error_user,
+password: wrong_password)</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>def test_wrong_password_username5(driver):</t>
+  </si>
+  <si>
+    <t>Användare lyckats inte att logga
+ in med fel lösenord. 
+(username:  visual_user,
+password: wrong_password)</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>def test_locked_user_givenpassword(driver):</t>
+  </si>
+  <si>
+    <t>Låsta användare kan inte logga in. 
+(username:  locked_out_user,
+password: secret_sauce)</t>
+  </si>
+  <si>
+    <t>#14</t>
+  </si>
+  <si>
+    <t>def test_locked_user_wrongpassword(driver):</t>
+  </si>
+  <si>
+    <t>Kontrollerar att låsta användarkonton inte kan logga in med 
+rätt lösenord, vilket är ett viktigt säkerhetskrav.</t>
+  </si>
+  <si>
+    <t>Kontrollerar att låsta användarkonton inte kan logga in med 
+fel lösenord, vilket är ett viktigt säkerhetskrav.</t>
+  </si>
+  <si>
+    <t>Låsta användare kan inte logga in. 
+(username:  locked_out_user,
+password: secret_sauc)</t>
+  </si>
+  <si>
+    <t>#15</t>
+  </si>
+  <si>
+    <t>def test_empty_fields(driver):</t>
+  </si>
+  <si>
+    <t>Validerar att inloggning inte tillåts när obligatoriska fält saknas.</t>
+  </si>
+  <si>
+    <t>Användare kan inte logga inte med
+tömma fälten.
+(username: tömma,
+password: tömma)</t>
+  </si>
+  <si>
+    <t>#16</t>
+  </si>
+  <si>
+    <t>def test_username_without_password(driver):</t>
+  </si>
+  <si>
+    <t>Användare kan inte logga inte med
+tömma lösenord fält.
+(username: standard_user,
+password: tömma)</t>
+  </si>
+  <si>
+    <t>#17</t>
+  </si>
+  <si>
+    <t>def test_password_without_username(driver):</t>
+  </si>
+  <si>
+    <t>Validerar att inloggning inte tillåts när användarnamn anges
+men lösenord saknas.</t>
+  </si>
+  <si>
+    <t>Validerar att inloggning inte tillåts när lösenord anges
+men användarnamn saknas.</t>
+  </si>
+  <si>
+    <t>Användare kan inte logga inte med
+tömma användarnamn fält.
+(username: tömma,
+password: secret_sauce)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +400,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -112,7 +453,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -120,16 +461,142 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -466,98 +933,838 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BBF6A0-D8E2-406A-AD12-25A43EEED0E6}">
-  <dimension ref="B2:Q5"/>
+  <dimension ref="A2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E2" s="2" t="s">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="20"/>
+    </row>
+    <row r="8" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="22"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="22"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
+    </row>
+    <row r="16" spans="1:17" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="22"/>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="22"/>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="22"/>
+    </row>
+    <row r="24" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="22"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25"/>
+    </row>
+    <row r="26" spans="1:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="22"/>
+    </row>
+    <row r="28" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="22"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="25"/>
+    </row>
+    <row r="30" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="27"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="25"/>
+    </row>
+    <row r="32" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="22"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="25"/>
+    </row>
+    <row r="34" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" s="22"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="25"/>
+    </row>
+    <row r="36" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="22"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="25"/>
+    </row>
+    <row r="38" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" s="22"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="25"/>
+    </row>
+    <row r="40" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J40" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E2:Q2"/>
+  <mergeCells count="39">
+    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="A8:B40"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C8:C40"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="A2:J3"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{0D70471D-5F48-46BB-A16F-FCF8C9ECB572}"/>
+    <hyperlink ref="C8" r:id="rId1" xr:uid="{0D70471D-5F48-46BB-A16F-FCF8C9ECB572}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test specification inloggningsfunktion och integrationstester updated
</commit_message>
<xml_diff>
--- a/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
+++ b/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studies\Testautomation_CI_CD\InlämningsUppgift_TA\Del_1-Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E184918-8B12-4AD7-BCD5-7EDF25989081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B4308D-699E-4373-8254-7851F9B069FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
   </bookViews>
@@ -533,70 +533,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -935,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BBF6A0-D8E2-406A-AD12-25A43EEED0E6}">
   <dimension ref="A2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40:J40"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,18 +956,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -977,16 +977,16 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -996,32 +996,32 @@
       <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="K4" s="5"/>
@@ -1033,30 +1033,30 @@
       <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="10" t="s">
         <v>29</v>
       </c>
       <c r="K5" s="5"/>
@@ -1068,16 +1068,16 @@
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1087,648 +1087,654 @@
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="20"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:17" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="22"/>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:17" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="25"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="22"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="27"/>
+      <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:17" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="22"/>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="22"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="26" t="s">
+      <c r="I18" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="27"/>
+      <c r="J18" s="24"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="22"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="26" t="s">
+      <c r="I20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="27"/>
+      <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="22"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="17" t="s">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="22"/>
+      <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="22"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="19"/>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="22"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="25"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="17" t="s">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="22"/>
+      <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="22"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="19"/>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17" t="s">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G28" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="21" t="s">
+      <c r="I28" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="22"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="25"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G30" s="18" t="s">
+      <c r="G30" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="H30" s="18" t="s">
+      <c r="H30" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="26" t="s">
+      <c r="I30" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="27"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="25"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="17" t="s">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="18" t="s">
+      <c r="F32" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="21" t="s">
+      <c r="I32" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J32" s="22"/>
+      <c r="J32" s="19"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="25"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="17" t="s">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="18" t="s">
+      <c r="G34" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H34" s="18" t="s">
+      <c r="H34" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="21" t="s">
+      <c r="I34" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="22"/>
+      <c r="J34" s="19"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="25"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17" t="s">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="21" t="s">
+      <c r="I36" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J36" s="22"/>
+      <c r="J36" s="19"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="25"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="17" t="s">
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F38" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="G38" s="18" t="s">
+      <c r="G38" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="21" t="s">
+      <c r="I38" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J38" s="22"/>
+      <c r="J38" s="19"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="25"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="17"/>
     </row>
     <row r="40" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="17" t="s">
+      <c r="A40" s="20"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G40" s="18" t="s">
+      <c r="G40" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="21" t="s">
+      <c r="I40" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J40" s="22"/>
+      <c r="J40" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="D37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="I36:J36"/>
+  <mergeCells count="40">
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="D25:J25"/>
     <mergeCell ref="A8:B40"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
@@ -1745,20 +1751,15 @@
     <mergeCell ref="D19:J19"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="C8:C40"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="D25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="D27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="I36:J36"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Test specs for Inloggningsfunktion and Integrationtester has been updated.
</commit_message>
<xml_diff>
--- a/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
+++ b/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studies\Testautomation_CI_CD\InlämningsUppgift_TA\Del_1-Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B4308D-699E-4373-8254-7851F9B069FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84890818-E18B-4571-8013-7BB960F839D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
   <si>
     <t xml:space="preserve">Test case ID </t>
   </si>
@@ -378,6 +378,19 @@
 tömma användarnamn fält.
 (username: tömma,
 password: secret_sauce)</t>
+  </si>
+  <si>
+    <t>#18</t>
+  </si>
+  <si>
+    <t>CI-Inloggningsfunktion</t>
+  </si>
+  <si>
+    <t>Kontrolleras att alla tester körs vid varje ändring som pushas eller vid
+ varje pull request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All tester körs och resultat loggas </t>
   </si>
 </sst>
 </file>
@@ -518,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -565,12 +578,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -579,18 +622,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -933,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BBF6A0-D8E2-406A-AD12-25A43EEED0E6}">
-  <dimension ref="A2:Q40"/>
+  <dimension ref="A2:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,18 +987,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -977,16 +1008,16 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -996,10 +1027,10 @@
       <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
@@ -1033,8 +1064,8 @@
       <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
@@ -1068,16 +1099,16 @@
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1087,10 +1118,10 @@
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
@@ -1109,16 +1140,16 @@
       <c r="H7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="22"/>
+      <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:17" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="26" t="s">
         <v>10</v>
       </c>
@@ -1137,26 +1168,26 @@
       <c r="H8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="19"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="26"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:17" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="26"/>
       <c r="D10" s="13" t="s">
         <v>33</v>
@@ -1173,26 +1204,26 @@
       <c r="H10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="19"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="17"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="29"/>
     </row>
     <row r="12" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="26"/>
       <c r="D12" s="13" t="s">
         <v>38</v>
@@ -1209,26 +1240,26 @@
       <c r="H12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="19"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="26"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="29"/>
     </row>
     <row r="14" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="26"/>
       <c r="D14" s="13" t="s">
         <v>41</v>
@@ -1245,26 +1276,26 @@
       <c r="H14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="24"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="26"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
     </row>
     <row r="16" spans="1:17" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="26"/>
       <c r="D16" s="13" t="s">
         <v>44</v>
@@ -1281,26 +1312,26 @@
       <c r="H16" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="26"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="19"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="23"/>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="26"/>
       <c r="D18" s="13" t="s">
         <v>47</v>
@@ -1317,26 +1348,26 @@
       <c r="H18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="24"/>
+      <c r="J18" s="25"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="26"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="19"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="23"/>
     </row>
     <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="26"/>
       <c r="D20" s="13" t="s">
         <v>51</v>
@@ -1353,26 +1384,26 @@
       <c r="H20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="24"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="26"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="19"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="26"/>
       <c r="D22" s="13" t="s">
         <v>54</v>
@@ -1389,26 +1420,26 @@
       <c r="H22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="26"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="19"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="23"/>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="26"/>
       <c r="D24" s="13" t="s">
         <v>58</v>
@@ -1425,26 +1456,26 @@
       <c r="H24" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="19"/>
+      <c r="J24" s="23"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="26"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="17"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="29"/>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="26"/>
       <c r="D26" s="13" t="s">
         <v>62</v>
@@ -1461,26 +1492,26 @@
       <c r="H26" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="19"/>
+      <c r="J26" s="23"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="26"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="19"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="23"/>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="26"/>
       <c r="D28" s="13" t="s">
         <v>65</v>
@@ -1497,26 +1528,26 @@
       <c r="H28" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="19"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="26"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="17"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="26"/>
       <c r="D30" s="13" t="s">
         <v>68</v>
@@ -1533,26 +1564,26 @@
       <c r="H30" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="24"/>
+      <c r="J30" s="25"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="26"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="17"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="29"/>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="26"/>
       <c r="D32" s="13" t="s">
         <v>71</v>
@@ -1569,26 +1600,26 @@
       <c r="H32" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="18" t="s">
+      <c r="I32" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J32" s="19"/>
+      <c r="J32" s="23"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="26"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="29"/>
     </row>
     <row r="34" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="26"/>
       <c r="D34" s="13" t="s">
         <v>74</v>
@@ -1605,26 +1636,26 @@
       <c r="H34" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="18" t="s">
+      <c r="I34" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="19"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="26"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="17"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="29"/>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="26"/>
       <c r="D36" s="13" t="s">
         <v>79</v>
@@ -1641,26 +1672,26 @@
       <c r="H36" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="18" t="s">
+      <c r="I36" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J36" s="19"/>
+      <c r="J36" s="23"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="26"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="17"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="29"/>
     </row>
     <row r="38" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="26"/>
       <c r="D38" s="13" t="s">
         <v>83</v>
@@ -1677,28 +1708,28 @@
       <c r="H38" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="18" t="s">
+      <c r="I38" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J38" s="19"/>
+      <c r="J38" s="23"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="17"/>
-    </row>
-    <row r="40" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
-      <c r="B40" s="20"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="29"/>
+    </row>
+    <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="26"/>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="15" t="s">
         <v>86</v>
       </c>
       <c r="E40" s="13" t="s">
@@ -1713,13 +1744,49 @@
       <c r="H40" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="18" t="s">
+      <c r="I40" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J40" s="19"/>
+      <c r="J40" s="23"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="1:10" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="J42" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
     <mergeCell ref="D31:J31"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A4:B5"/>
@@ -1735,22 +1802,21 @@
     <mergeCell ref="D23:J23"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="D25:J25"/>
-    <mergeCell ref="A8:B40"/>
+    <mergeCell ref="A8:B42"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="D11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="I16:J16"/>
     <mergeCell ref="D17:J17"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="D19:J19"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C8:C40"/>
+    <mergeCell ref="C8:C42"/>
     <mergeCell ref="D37:J37"/>
     <mergeCell ref="I38:J38"/>
     <mergeCell ref="D39:J39"/>
@@ -1760,6 +1826,8 @@
     <mergeCell ref="I34:J34"/>
     <mergeCell ref="D35:J35"/>
     <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Test specs for Inloggningsfunktion  has been updated.
</commit_message>
<xml_diff>
--- a/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
+++ b/Del_1-Rapport/Test_Specifikation_Inloggningsfunktion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studies\Testautomation_CI_CD\InlämningsUppgift_TA\Del_1-Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84890818-E18B-4571-8013-7BB960F839D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF57927-46D6-4B29-A38C-93BF9FE6E09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F97E49E7-5B5D-407D-92EB-A7BB87B04C5F}"/>
   </bookViews>
@@ -383,14 +383,14 @@
     <t>#18</t>
   </si>
   <si>
-    <t>CI-Inloggningsfunktion</t>
-  </si>
-  <si>
     <t>Kontrolleras att alla tester körs vid varje ändring som pushas eller vid
  varje pull request</t>
   </si>
   <si>
     <t xml:space="preserve">All tester körs och resultat loggas </t>
+  </si>
+  <si>
+    <t>Test_CI-Inloggningsfunktion</t>
   </si>
 </sst>
 </file>
@@ -588,46 +588,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BBF6A0-D8E2-406A-AD12-25A43EEED0E6}">
   <dimension ref="A2:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,18 +987,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -1008,16 +1008,16 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -1027,10 +1027,10 @@
       <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
@@ -1064,8 +1064,8 @@
       <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
@@ -1099,16 +1099,16 @@
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1118,10 +1118,10 @@
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
@@ -1140,17 +1140,17 @@
       <c r="H7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="32"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:17" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -1168,27 +1168,27 @@
       <c r="H8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="23"/>
+      <c r="J8" s="29"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:17" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="13" t="s">
         <v>33</v>
       </c>
@@ -1204,27 +1204,27 @@
       <c r="H10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="23"/>
+      <c r="J10" s="29"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="29"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="13" t="s">
         <v>38</v>
       </c>
@@ -1240,27 +1240,27 @@
       <c r="H12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="23"/>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
     </row>
     <row r="14" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="13" t="s">
         <v>41</v>
       </c>
@@ -1276,27 +1276,27 @@
       <c r="H14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16" spans="1:17" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="26"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="13" t="s">
         <v>44</v>
       </c>
@@ -1312,27 +1312,27 @@
       <c r="H16" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="23"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="13" t="s">
         <v>47</v>
       </c>
@@ -1348,27 +1348,27 @@
       <c r="H18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="25"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="26"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="13" t="s">
         <v>51</v>
       </c>
@@ -1384,27 +1384,27 @@
       <c r="H20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="25"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="23"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="29"/>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="26"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="13" t="s">
         <v>54</v>
       </c>
@@ -1420,27 +1420,27 @@
       <c r="H22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="23"/>
+      <c r="J22" s="29"/>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="29"/>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="13" t="s">
         <v>58</v>
       </c>
@@ -1456,27 +1456,27 @@
       <c r="H24" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="23"/>
+      <c r="J24" s="29"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="29"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="23"/>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="26"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="13" t="s">
         <v>62</v>
       </c>
@@ -1492,27 +1492,27 @@
       <c r="H26" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="23"/>
+      <c r="J26" s="29"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="23"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="29"/>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="26"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="13" t="s">
         <v>65</v>
       </c>
@@ -1528,27 +1528,27 @@
       <c r="H28" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="21" t="s">
+      <c r="I28" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="23"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="29"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="26"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="13" t="s">
         <v>68</v>
       </c>
@@ -1564,27 +1564,27 @@
       <c r="H30" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="24" t="s">
+      <c r="I30" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="25"/>
+      <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="29"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="23"/>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="26"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34"/>
       <c r="D32" s="13" t="s">
         <v>71</v>
       </c>
@@ -1600,27 +1600,27 @@
       <c r="H32" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="21" t="s">
+      <c r="I32" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J32" s="23"/>
+      <c r="J32" s="29"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="23"/>
     </row>
     <row r="34" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="26"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="34"/>
       <c r="D34" s="13" t="s">
         <v>74</v>
       </c>
@@ -1636,27 +1636,27 @@
       <c r="H34" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="21" t="s">
+      <c r="I34" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="23"/>
+      <c r="J34" s="29"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="29"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="23"/>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="26"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
       <c r="D36" s="13" t="s">
         <v>79</v>
       </c>
@@ -1672,27 +1672,27 @@
       <c r="H36" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="21" t="s">
+      <c r="I36" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J36" s="23"/>
+      <c r="J36" s="29"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="29"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="23"/>
     </row>
     <row r="38" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="26"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="13" t="s">
         <v>83</v>
       </c>
@@ -1708,27 +1708,27 @@
       <c r="H38" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="21" t="s">
+      <c r="I38" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J38" s="23"/>
+      <c r="J38" s="29"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="29"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="23"/>
     </row>
     <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="26"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34"/>
       <c r="D40" s="15" t="s">
         <v>86</v>
       </c>
@@ -1744,15 +1744,15 @@
       <c r="H40" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="21" t="s">
+      <c r="I40" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J40" s="23"/>
+      <c r="J40" s="29"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="26"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
       <c r="D41" s="15"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
@@ -1762,31 +1762,56 @@
       <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:10" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="26"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="34"/>
       <c r="D42" s="18" t="s">
         <v>91</v>
       </c>
       <c r="E42" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F42" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="G42" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>94</v>
       </c>
       <c r="H42" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I42" s="30" t="s">
+      <c r="I42" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="J42" s="30"/>
+      <c r="J42" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C8:C42"/>
+    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="D11:J11"/>
     <mergeCell ref="D31:J31"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A4:B5"/>
@@ -1803,31 +1828,6 @@
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="D25:J25"/>
     <mergeCell ref="A8:B42"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C8:C42"/>
-    <mergeCell ref="D37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>